<commit_message>
SSC Boxplots and QvsC
added options for separating stormflow and baseflow, totally changes the
boxplots and Q vs C plots
</commit_message>
<xml_diff>
--- a/Data/T/SyntheticRatingCurve/SyntheticRatingCurve.xlsx
+++ b/Data/T/SyntheticRatingCurve/SyntheticRatingCurve.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="LBJ_SRC" sheetId="1" r:id="rId1"/>
@@ -854,10 +854,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,41 +902,32 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>AVERAGE(N2_SRC!A8:A9)</f>
-        <v>8.8449999999999989</v>
-      </c>
-      <c r="C2" s="1">
-        <f>AVERAGE(N2_SRC!B8:B9)</f>
-        <v>8.8699999999999992</v>
-      </c>
-      <c r="D2" s="1">
-        <f>AVERAGE(N2_SRC!C8:C9)</f>
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="E2" s="1">
-        <f>AVERAGE(N2_SRC!D8:D9)</f>
-        <v>8.6150000000000002</v>
-      </c>
-      <c r="F2" s="1">
-        <f>AVERAGE(N2_SRC!E8:E9)</f>
-        <v>9.2149999999999999</v>
-      </c>
-      <c r="G2" s="1">
-        <f>AVERAGE(N2_SRC!F8:F9)</f>
-        <v>14.79</v>
-      </c>
-      <c r="H2" s="1">
-        <f>AVERAGE(N2_SRC!G8:G9)</f>
-        <v>14.969999999999999</v>
-      </c>
-      <c r="I2" s="1">
-        <f>AVERAGE(N2_SRC!H8:H9)</f>
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>1.9047619047619047</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -944,40 +935,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <f>AVERAGE(N2_SRC!A11:A13)</f>
-        <v>104.99000000000001</v>
+        <f>AVERAGE(N2_SRC!A8:A9)</f>
+        <v>8.8449999999999989</v>
       </c>
       <c r="C3" s="1">
-        <f>AVERAGE(N2_SRC!B11:B13)</f>
-        <v>105.19666666666667</v>
+        <f>AVERAGE(N2_SRC!B8:B9)</f>
+        <v>8.8699999999999992</v>
       </c>
       <c r="D3" s="1">
-        <f>AVERAGE(N2_SRC!C11:C13)</f>
-        <v>3.34</v>
+        <f>AVERAGE(N2_SRC!C8:C9)</f>
+        <v>0.13600000000000001</v>
       </c>
       <c r="E3" s="1">
-        <f>AVERAGE(N2_SRC!D11:D13)</f>
-        <v>98.84333333333332</v>
+        <f>AVERAGE(N2_SRC!D8:D9)</f>
+        <v>8.6150000000000002</v>
       </c>
       <c r="F3" s="1">
-        <f>AVERAGE(N2_SRC!E11:E13)</f>
-        <v>112.7</v>
+        <f>AVERAGE(N2_SRC!E8:E9)</f>
+        <v>9.2149999999999999</v>
       </c>
       <c r="G3" s="1">
-        <f>AVERAGE(N2_SRC!F11:F13)</f>
-        <v>190.78666666666666</v>
+        <f>AVERAGE(N2_SRC!F8:F9)</f>
+        <v>14.79</v>
       </c>
       <c r="H3" s="1">
-        <f>AVERAGE(N2_SRC!G11:G13)</f>
-        <v>191.74333333333334</v>
+        <f>AVERAGE(N2_SRC!G8:G9)</f>
+        <v>14.969999999999999</v>
       </c>
       <c r="I3" s="1">
-        <f>AVERAGE(N2_SRC!H11:H13)</f>
-        <v>9.43</v>
+        <f>AVERAGE(N2_SRC!H8:H9)</f>
+        <v>0.61499999999999999</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1">
-        <v>80</v>
+        <v>1.9047619047619047</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -985,40 +976,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGE(N2_SRC!A15:A16)</f>
-        <v>350.14499999999998</v>
+        <f>AVERAGE(N2_SRC!A11:A13)</f>
+        <v>104.99000000000001</v>
       </c>
       <c r="C4" s="1">
-        <f>AVERAGE(N2_SRC!B15:B16)</f>
-        <v>350.90499999999997</v>
+        <f>AVERAGE(N2_SRC!B11:B13)</f>
+        <v>105.19666666666667</v>
       </c>
       <c r="D4" s="1">
-        <f>AVERAGE(N2_SRC!C15:C16)</f>
-        <v>8.6300000000000008</v>
+        <f>AVERAGE(N2_SRC!C11:C13)</f>
+        <v>3.34</v>
       </c>
       <c r="E4" s="1">
-        <f>AVERAGE(N2_SRC!D15:D16)</f>
-        <v>333.39499999999998</v>
+        <f>AVERAGE(N2_SRC!D11:D13)</f>
+        <v>98.84333333333332</v>
       </c>
       <c r="F4" s="1">
-        <f>AVERAGE(N2_SRC!E15:E16)</f>
-        <v>367.94499999999999</v>
+        <f>AVERAGE(N2_SRC!E11:E13)</f>
+        <v>112.7</v>
       </c>
       <c r="G4" s="1">
-        <f>AVERAGE(N2_SRC!F15:F16)</f>
-        <v>693.06</v>
+        <f>AVERAGE(N2_SRC!F11:F13)</f>
+        <v>190.78666666666666</v>
       </c>
       <c r="H4" s="1">
-        <f>AVERAGE(N2_SRC!G15:G16)</f>
-        <v>697.61</v>
+        <f>AVERAGE(N2_SRC!G11:G13)</f>
+        <v>191.74333333333334</v>
       </c>
       <c r="I4" s="1">
-        <f>AVERAGE(N2_SRC!H15:H16)</f>
-        <v>25.14</v>
+        <f>AVERAGE(N2_SRC!H11:H13)</f>
+        <v>9.43</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1">
-        <v>550</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1026,40 +1017,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGE(N2_SRC!A18:A19)</f>
-        <v>612.05500000000006</v>
+        <f>AVERAGE(N2_SRC!A15:A16)</f>
+        <v>350.14499999999998</v>
       </c>
       <c r="C5" s="1">
-        <f>AVERAGE(N2_SRC!B18:B19)</f>
-        <v>610.95500000000004</v>
+        <f>AVERAGE(N2_SRC!B15:B16)</f>
+        <v>350.90499999999997</v>
       </c>
       <c r="D5" s="1">
-        <f>AVERAGE(N2_SRC!C18:C19)</f>
-        <v>7.8999999999999995</v>
+        <f>AVERAGE(N2_SRC!C15:C16)</f>
+        <v>8.6300000000000008</v>
       </c>
       <c r="E5" s="1">
-        <f>AVERAGE(N2_SRC!D18:D19)</f>
-        <v>591.48500000000001</v>
+        <f>AVERAGE(N2_SRC!D15:D16)</f>
+        <v>333.39499999999998</v>
       </c>
       <c r="F5" s="1">
-        <f>AVERAGE(N2_SRC!E18:E19)</f>
-        <v>626.1400000000001</v>
+        <f>AVERAGE(N2_SRC!E15:E16)</f>
+        <v>367.94499999999999</v>
       </c>
       <c r="G5" s="1">
-        <f>AVERAGE(N2_SRC!F18:F19)</f>
-        <v>2443.9850000000001</v>
+        <f>AVERAGE(N2_SRC!F15:F16)</f>
+        <v>693.06</v>
       </c>
       <c r="H5" s="1">
-        <f>AVERAGE(N2_SRC!G18:G19)</f>
-        <v>2403.3150000000001</v>
+        <f>AVERAGE(N2_SRC!G15:G16)</f>
+        <v>697.61</v>
       </c>
       <c r="I5" s="1">
-        <f>AVERAGE(N2_SRC!H18:H19)</f>
-        <v>216.815</v>
+        <f>AVERAGE(N2_SRC!H15:H16)</f>
+        <v>25.14</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
-        <v>840</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1067,39 +1058,80 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
+        <f>AVERAGE(N2_SRC!A18:A19)</f>
+        <v>612.05500000000006</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(N2_SRC!B18:B19)</f>
+        <v>610.95500000000004</v>
+      </c>
+      <c r="D6" s="1">
+        <f>AVERAGE(N2_SRC!C18:C19)</f>
+        <v>7.8999999999999995</v>
+      </c>
+      <c r="E6" s="1">
+        <f>AVERAGE(N2_SRC!D18:D19)</f>
+        <v>591.48500000000001</v>
+      </c>
+      <c r="F6" s="1">
+        <f>AVERAGE(N2_SRC!E18:E19)</f>
+        <v>626.1400000000001</v>
+      </c>
+      <c r="G6" s="1">
+        <f>AVERAGE(N2_SRC!F18:F19)</f>
+        <v>2443.9850000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <f>AVERAGE(N2_SRC!G18:G19)</f>
+        <v>2403.3150000000001</v>
+      </c>
+      <c r="I6" s="1">
+        <f>AVERAGE(N2_SRC!H18:H19)</f>
+        <v>216.815</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <f>AVERAGE(N2_SRC!A2:A21)</f>
         <v>301.803</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <f>AVERAGE(N2_SRC!B2:B21)</f>
         <v>301.77100000000002</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <f>AVERAGE(N2_SRC!C2:C21)</f>
         <v>7.1362000000000005</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <f>AVERAGE(N2_SRC!D2:D21)</f>
         <v>286.49200000000002</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <f>AVERAGE(N2_SRC!E2:E21)</f>
         <v>315.06000000000006</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
         <f>AVERAGE(N2_SRC!F2:F21)</f>
         <v>1075.4970000000001</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H7" s="1">
         <f>AVERAGE(N2_SRC!G2:G21)</f>
         <v>1075.056</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I7" s="1">
         <f>AVERAGE(N2_SRC!H2:H21)</f>
         <v>96.678000000000011</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
         <v>1492.8571428571427</v>
       </c>
     </row>
@@ -1111,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,41 +1191,32 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>AVERAGE(LBJ_SRC!A8:A9)</f>
-        <v>14.004999999999999</v>
-      </c>
-      <c r="C2" s="1">
-        <f>AVERAGE(LBJ_SRC!B8:B9)</f>
-        <v>15.170000000000002</v>
-      </c>
-      <c r="D2" s="1">
-        <f>AVERAGE(LBJ_SRC!C8:C9)</f>
-        <v>3.1749999999999998</v>
-      </c>
-      <c r="E2" s="1">
-        <f>AVERAGE(LBJ_SRC!D8:D9)</f>
-        <v>11.865</v>
-      </c>
-      <c r="F2" s="1">
-        <f>AVERAGE(LBJ_SRC!E8:E9)</f>
-        <v>26.93</v>
-      </c>
-      <c r="G2" s="1">
-        <f>AVERAGE(LBJ_SRC!F8:F9)</f>
-        <v>27.53</v>
-      </c>
-      <c r="H2" s="1">
-        <f>AVERAGE(LBJ_SRC!G8:G9)</f>
-        <v>29.86</v>
-      </c>
-      <c r="I2" s="1">
-        <f>AVERAGE(LBJ_SRC!H8:H9)</f>
-        <v>8.43</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>8.8888888888888893</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1201,40 +1224,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <f>AVERAGE(LBJ_SRC!A11:A12)</f>
-        <v>118.375</v>
+        <f>AVERAGE(LBJ_SRC!A8:A9)</f>
+        <v>14.004999999999999</v>
       </c>
       <c r="C3" s="1">
-        <f>AVERAGE(LBJ_SRC!B11:B12)</f>
-        <v>118.33500000000001</v>
+        <f>AVERAGE(LBJ_SRC!B8:B9)</f>
+        <v>15.170000000000002</v>
       </c>
       <c r="D3" s="1">
-        <f>AVERAGE(LBJ_SRC!C11:C12)</f>
-        <v>3.1</v>
+        <f>AVERAGE(LBJ_SRC!C8:C9)</f>
+        <v>3.1749999999999998</v>
       </c>
       <c r="E3" s="1">
-        <f>AVERAGE(LBJ_SRC!D11:D12)</f>
-        <v>111.825</v>
+        <f>AVERAGE(LBJ_SRC!D8:D9)</f>
+        <v>11.865</v>
       </c>
       <c r="F3" s="1">
-        <f>AVERAGE(LBJ_SRC!E11:E12)</f>
-        <v>129.07499999999999</v>
+        <f>AVERAGE(LBJ_SRC!E8:E9)</f>
+        <v>26.93</v>
       </c>
       <c r="G3" s="1">
-        <f>AVERAGE(LBJ_SRC!F11:F12)</f>
-        <v>232.715</v>
+        <f>AVERAGE(LBJ_SRC!F8:F9)</f>
+        <v>27.53</v>
       </c>
       <c r="H3" s="1">
-        <f>AVERAGE(LBJ_SRC!G11:G12)</f>
-        <v>235.01499999999999</v>
+        <f>AVERAGE(LBJ_SRC!G8:G9)</f>
+        <v>29.86</v>
       </c>
       <c r="I3" s="1">
-        <f>AVERAGE(LBJ_SRC!H11:H12)</f>
-        <v>15.815000000000001</v>
+        <f>AVERAGE(LBJ_SRC!H8:H9)</f>
+        <v>8.43</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1">
-        <v>248.88888888888889</v>
+        <v>8.8888888888888893</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1242,40 +1265,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGE(LBJ_SRC!A14:A15)</f>
-        <v>272.065</v>
+        <f>AVERAGE(LBJ_SRC!A11:A12)</f>
+        <v>118.375</v>
       </c>
       <c r="C4" s="1">
-        <f>AVERAGE(LBJ_SRC!B14:B15)</f>
-        <v>274.20999999999998</v>
+        <f>AVERAGE(LBJ_SRC!B11:B12)</f>
+        <v>118.33500000000001</v>
       </c>
       <c r="D4" s="1">
-        <f>AVERAGE(LBJ_SRC!C14:C15)</f>
-        <v>6.5050000000000008</v>
+        <f>AVERAGE(LBJ_SRC!C11:C12)</f>
+        <v>3.1</v>
       </c>
       <c r="E4" s="1">
-        <f>AVERAGE(LBJ_SRC!D14:D15)</f>
-        <v>264.07</v>
+        <f>AVERAGE(LBJ_SRC!D11:D12)</f>
+        <v>111.825</v>
       </c>
       <c r="F4" s="1">
-        <f>AVERAGE(LBJ_SRC!E14:E15)</f>
-        <v>286.625</v>
+        <f>AVERAGE(LBJ_SRC!E11:E12)</f>
+        <v>129.07499999999999</v>
       </c>
       <c r="G4" s="1">
-        <f>AVERAGE(LBJ_SRC!F14:F15)</f>
-        <v>600.38499999999999</v>
+        <f>AVERAGE(LBJ_SRC!F11:F12)</f>
+        <v>232.715</v>
       </c>
       <c r="H4" s="1">
-        <f>AVERAGE(LBJ_SRC!G14:G15)</f>
-        <v>607.26</v>
+        <f>AVERAGE(LBJ_SRC!G11:G12)</f>
+        <v>235.01499999999999</v>
       </c>
       <c r="I4" s="1">
-        <f>AVERAGE(LBJ_SRC!H14:H15)</f>
-        <v>21.454999999999998</v>
+        <f>AVERAGE(LBJ_SRC!H11:H12)</f>
+        <v>15.815000000000001</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1">
-        <v>928.57142857142867</v>
+        <v>248.88888888888889</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1283,40 +1306,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGE(LBJ_SRC!A17:A18)</f>
-        <v>621.52499999999998</v>
+        <f>AVERAGE(LBJ_SRC!A14:A15)</f>
+        <v>272.065</v>
       </c>
       <c r="C5" s="1">
-        <f>AVERAGE(LBJ_SRC!B17:B18)</f>
-        <v>619.52500000000009</v>
+        <f>AVERAGE(LBJ_SRC!B14:B15)</f>
+        <v>274.20999999999998</v>
       </c>
       <c r="D5" s="1">
-        <f>AVERAGE(LBJ_SRC!C17:C18)</f>
-        <v>31.299999999999997</v>
+        <f>AVERAGE(LBJ_SRC!C14:C15)</f>
+        <v>6.5050000000000008</v>
       </c>
       <c r="E5" s="1">
-        <f>AVERAGE(LBJ_SRC!D17:D18)</f>
-        <v>521.76</v>
+        <f>AVERAGE(LBJ_SRC!D14:D15)</f>
+        <v>264.07</v>
       </c>
       <c r="F5" s="1">
-        <f>AVERAGE(LBJ_SRC!E17:E18)</f>
-        <v>593.08500000000004</v>
+        <f>AVERAGE(LBJ_SRC!E14:E15)</f>
+        <v>286.625</v>
       </c>
       <c r="G5" s="1">
-        <f>AVERAGE(LBJ_SRC!F17:F18)</f>
-        <v>1580.4650000000001</v>
+        <f>AVERAGE(LBJ_SRC!F14:F15)</f>
+        <v>600.38499999999999</v>
       </c>
       <c r="H5" s="1">
-        <f>AVERAGE(LBJ_SRC!G17:G18)</f>
-        <v>1590.635</v>
+        <f>AVERAGE(LBJ_SRC!G14:G15)</f>
+        <v>607.26</v>
       </c>
       <c r="I5" s="1">
-        <f>AVERAGE(LBJ_SRC!H17:H18)</f>
-        <v>129.125</v>
+        <f>AVERAGE(LBJ_SRC!H14:H15)</f>
+        <v>21.454999999999998</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
-        <v>2729.411764705882</v>
+        <v>928.57142857142867</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1324,39 +1347,80 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
+        <f>AVERAGE(LBJ_SRC!A17:A18)</f>
+        <v>621.52499999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(LBJ_SRC!B17:B18)</f>
+        <v>619.52500000000009</v>
+      </c>
+      <c r="D6" s="1">
+        <f>AVERAGE(LBJ_SRC!C17:C18)</f>
+        <v>31.299999999999997</v>
+      </c>
+      <c r="E6" s="1">
+        <f>AVERAGE(LBJ_SRC!D17:D18)</f>
+        <v>521.76</v>
+      </c>
+      <c r="F6" s="1">
+        <f>AVERAGE(LBJ_SRC!E17:E18)</f>
+        <v>593.08500000000004</v>
+      </c>
+      <c r="G6" s="1">
+        <f>AVERAGE(LBJ_SRC!F17:F18)</f>
+        <v>1580.4650000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <f>AVERAGE(LBJ_SRC!G17:G18)</f>
+        <v>1590.635</v>
+      </c>
+      <c r="I6" s="1">
+        <f>AVERAGE(LBJ_SRC!H17:H18)</f>
+        <v>129.125</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>2729.411764705882</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <f>AVERAGE(LBJ_SRC!A20:A22)</f>
         <v>451.54333333333335</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <f>AVERAGE(LBJ_SRC!B20:B22)</f>
         <v>447.48</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <f>AVERAGE(LBJ_SRC!C20:C22)</f>
         <v>33.853333333333332</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <f>AVERAGE(LBJ_SRC!D20:D22)</f>
         <v>386.56666666666666</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <f>AVERAGE(LBJ_SRC!E20:E22)</f>
         <v>506.96</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
         <f>AVERAGE(LBJ_SRC!F20:F22)</f>
         <v>847.47333333333336</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H7" s="1">
         <f>AVERAGE(LBJ_SRC!G20:G22)</f>
         <v>854.36333333333334</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I7" s="1">
         <f>AVERAGE(LBJ_SRC!H20:H22)</f>
         <v>109.90333333333332</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
         <v>5467.6923076923076</v>
       </c>
     </row>
@@ -1777,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,41 +1889,32 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>AVERAGE(QUARRY_SRC!A8:A9)</f>
-        <v>6.7050000000000001</v>
-      </c>
-      <c r="C2" s="1">
-        <f>AVERAGE(QUARRY_SRC!B8:B9)</f>
-        <v>7.085</v>
-      </c>
-      <c r="D2" s="1">
-        <f>AVERAGE(QUARRY_SRC!C8:C9)</f>
-        <v>0.97</v>
-      </c>
-      <c r="E2" s="1">
-        <f>AVERAGE(QUARRY_SRC!D8:D9)</f>
-        <v>5.875</v>
-      </c>
-      <c r="F2" s="1">
-        <f>AVERAGE(QUARRY_SRC!E8:E9)</f>
-        <v>9.5850000000000009</v>
-      </c>
-      <c r="G2" s="1">
-        <f>AVERAGE(QUARRY_SRC!F8:F9)</f>
-        <v>13.384999999999998</v>
-      </c>
-      <c r="H2" s="1">
-        <f>AVERAGE(QUARRY_SRC!G8:G9)</f>
-        <v>13.530000000000001</v>
-      </c>
-      <c r="I2" s="1">
-        <f>AVERAGE(QUARRY_SRC!H8:H9)</f>
-        <v>3.91</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>4.2105263157894735</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1867,40 +1922,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <f>AVERAGE(QUARRY_SRC!A11:A12)</f>
-        <v>52.14</v>
+        <f>AVERAGE(QUARRY_SRC!A8:A9)</f>
+        <v>6.7050000000000001</v>
       </c>
       <c r="C3" s="1">
-        <f>AVERAGE(QUARRY_SRC!B11:B12)</f>
-        <v>52.7</v>
+        <f>AVERAGE(QUARRY_SRC!B8:B9)</f>
+        <v>7.085</v>
       </c>
       <c r="D3" s="1">
-        <f>AVERAGE(QUARRY_SRC!C11:C12)</f>
-        <v>3.395</v>
+        <f>AVERAGE(QUARRY_SRC!C8:C9)</f>
+        <v>0.97</v>
       </c>
       <c r="E3" s="1">
-        <f>AVERAGE(QUARRY_SRC!D11:D12)</f>
-        <v>46.34</v>
+        <f>AVERAGE(QUARRY_SRC!D8:D9)</f>
+        <v>5.875</v>
       </c>
       <c r="F3" s="1">
-        <f>AVERAGE(QUARRY_SRC!E11:E12)</f>
-        <v>61.994999999999997</v>
+        <f>AVERAGE(QUARRY_SRC!E8:E9)</f>
+        <v>9.5850000000000009</v>
       </c>
       <c r="G3" s="1">
-        <f>AVERAGE(QUARRY_SRC!F11:F12)</f>
-        <v>107.11500000000001</v>
+        <f>AVERAGE(QUARRY_SRC!F8:F9)</f>
+        <v>13.384999999999998</v>
       </c>
       <c r="H3" s="1">
-        <f>AVERAGE(QUARRY_SRC!G11:G12)</f>
-        <v>107.78999999999999</v>
+        <f>AVERAGE(QUARRY_SRC!G8:G9)</f>
+        <v>13.530000000000001</v>
       </c>
       <c r="I3" s="1">
-        <f>AVERAGE(QUARRY_SRC!H11:H12)</f>
-        <v>10.245000000000001</v>
+        <f>AVERAGE(QUARRY_SRC!H8:H9)</f>
+        <v>3.91</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1">
-        <v>157.89473684210526</v>
+        <v>4.2105263157894735</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1908,40 +1963,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGE(QUARRY_SRC!A14:A15)</f>
-        <v>218.875</v>
+        <f>AVERAGE(QUARRY_SRC!A11:A12)</f>
+        <v>52.14</v>
       </c>
       <c r="C4" s="1">
-        <f>AVERAGE(QUARRY_SRC!B14:B15)</f>
-        <v>222.86</v>
+        <f>AVERAGE(QUARRY_SRC!B11:B12)</f>
+        <v>52.7</v>
       </c>
       <c r="D4" s="1">
-        <f>AVERAGE(QUARRY_SRC!C14:C15)</f>
-        <v>18.73</v>
+        <f>AVERAGE(QUARRY_SRC!C11:C12)</f>
+        <v>3.395</v>
       </c>
       <c r="E4" s="1">
-        <f>AVERAGE(QUARRY_SRC!D14:D15)</f>
-        <v>201.56</v>
+        <f>AVERAGE(QUARRY_SRC!D11:D12)</f>
+        <v>46.34</v>
       </c>
       <c r="F4" s="1">
-        <f>AVERAGE(QUARRY_SRC!E14:E15)</f>
-        <v>327.75</v>
+        <f>AVERAGE(QUARRY_SRC!E11:E12)</f>
+        <v>61.994999999999997</v>
       </c>
       <c r="G4" s="1">
-        <f>AVERAGE(QUARRY_SRC!F14:F15)</f>
-        <v>548.19500000000005</v>
+        <f>AVERAGE(QUARRY_SRC!F11:F12)</f>
+        <v>107.11500000000001</v>
       </c>
       <c r="H4" s="1">
-        <f>AVERAGE(QUARRY_SRC!G14:G15)</f>
-        <v>558.81999999999994</v>
+        <f>AVERAGE(QUARRY_SRC!G11:G12)</f>
+        <v>107.78999999999999</v>
       </c>
       <c r="I4" s="1">
-        <f>AVERAGE(QUARRY_SRC!H14:H15)</f>
-        <v>52.493500000000004</v>
+        <f>AVERAGE(QUARRY_SRC!H11:H12)</f>
+        <v>10.245000000000001</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1">
-        <v>915.78947368421052</v>
+        <v>157.89473684210526</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1949,40 +2004,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGE(QUARRY_SRC!A17)</f>
-        <v>343.99</v>
+        <f>AVERAGE(QUARRY_SRC!A14:A15)</f>
+        <v>218.875</v>
       </c>
       <c r="C5" s="1">
-        <f>AVERAGE(QUARRY_SRC!B17)</f>
-        <v>351.69</v>
+        <f>AVERAGE(QUARRY_SRC!B14:B15)</f>
+        <v>222.86</v>
       </c>
       <c r="D5" s="1">
-        <f>AVERAGE(QUARRY_SRC!C17)</f>
-        <v>34.36</v>
+        <f>AVERAGE(QUARRY_SRC!C14:C15)</f>
+        <v>18.73</v>
       </c>
       <c r="E5" s="1">
-        <f>AVERAGE(QUARRY_SRC!D17)</f>
-        <v>297.66000000000003</v>
+        <f>AVERAGE(QUARRY_SRC!D14:D15)</f>
+        <v>201.56</v>
       </c>
       <c r="F5" s="1">
-        <f>AVERAGE(QUARRY_SRC!E17)</f>
-        <v>442.5</v>
+        <f>AVERAGE(QUARRY_SRC!E14:E15)</f>
+        <v>327.75</v>
       </c>
       <c r="G5" s="1">
-        <f>AVERAGE(QUARRY_SRC!F17)</f>
-        <v>783.59</v>
+        <f>AVERAGE(QUARRY_SRC!F14:F15)</f>
+        <v>548.19500000000005</v>
       </c>
       <c r="H5" s="1">
-        <f>AVERAGE(QUARRY_SRC!G17)</f>
-        <v>1612.58</v>
+        <f>AVERAGE(QUARRY_SRC!G14:G15)</f>
+        <v>558.81999999999994</v>
       </c>
       <c r="I5" s="1">
-        <f>AVERAGE(QUARRY_SRC!H17)</f>
-        <v>1723.94</v>
+        <f>AVERAGE(QUARRY_SRC!H14:H15)</f>
+        <v>52.493500000000004</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
-        <v>3151.1111111111109</v>
+        <v>915.78947368421052</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1990,39 +2045,80 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
+        <f>AVERAGE(QUARRY_SRC!A17)</f>
+        <v>343.99</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(QUARRY_SRC!B17)</f>
+        <v>351.69</v>
+      </c>
+      <c r="D6" s="1">
+        <f>AVERAGE(QUARRY_SRC!C17)</f>
+        <v>34.36</v>
+      </c>
+      <c r="E6" s="1">
+        <f>AVERAGE(QUARRY_SRC!D17)</f>
+        <v>297.66000000000003</v>
+      </c>
+      <c r="F6" s="1">
+        <f>AVERAGE(QUARRY_SRC!E17)</f>
+        <v>442.5</v>
+      </c>
+      <c r="G6" s="1">
+        <f>AVERAGE(QUARRY_SRC!F17)</f>
+        <v>783.59</v>
+      </c>
+      <c r="H6" s="1">
+        <f>AVERAGE(QUARRY_SRC!G17)</f>
+        <v>1612.58</v>
+      </c>
+      <c r="I6" s="1">
+        <f>AVERAGE(QUARRY_SRC!H17)</f>
+        <v>1723.94</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>3151.1111111111109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <f>AVERAGE(QUARRY_SRC!A19:A23)</f>
         <v>470.11399999999992</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <f>AVERAGE(QUARRY_SRC!B19:B23)</f>
         <v>471.18600000000004</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <f>AVERAGE(QUARRY_SRC!C19:C23)</f>
         <v>23.922000000000001</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <f>AVERAGE(QUARRY_SRC!D19:D23)</f>
         <v>418.65200000000004</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <f>AVERAGE(QUARRY_SRC!E19:E23)</f>
         <v>517.77800000000002</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
         <f>AVERAGE(QUARRY_SRC!F19:F23)</f>
         <v>2745.654</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H7" s="1">
         <f>AVERAGE(QUARRY_SRC!G19:G23)</f>
         <v>2791.0360000000001</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I7" s="1">
         <f>AVERAGE(QUARRY_SRC!H19:H23)</f>
         <v>449.79200000000003</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
         <v>7846.1538461538457</v>
       </c>
     </row>
@@ -2124,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2183,10 +2279,10 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>78</v>
-      </c>
-      <c r="K3" s="1">
-        <v>2.2222222222222223</v>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2194,10 +2290,10 @@
         <v>2</v>
       </c>
       <c r="H4">
-        <v>302</v>
+        <v>78</v>
       </c>
       <c r="K4" s="1">
-        <v>162.5</v>
+        <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2205,10 +2301,10 @@
         <v>3</v>
       </c>
       <c r="H5">
-        <v>658</v>
+        <v>302</v>
       </c>
       <c r="K5" s="1">
-        <v>1394.2857142857144</v>
+        <v>162.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2216,10 +2312,10 @@
         <v>4</v>
       </c>
       <c r="H6">
-        <v>1139</v>
+        <v>658</v>
       </c>
       <c r="K6" s="1">
-        <v>3651.4285714285716</v>
+        <v>1394.2857142857144</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2227,9 +2323,20 @@
         <v>5</v>
       </c>
       <c r="H7">
+        <v>1139</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3651.4285714285716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="H8">
         <v>1368</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K8" s="1">
         <v>3940.0000000000005</v>
       </c>
     </row>
@@ -2600,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,41 +2755,32 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>AVERAGE(N1_SRC!A8:A9)</f>
-        <v>7.9450000000000003</v>
-      </c>
-      <c r="C2" s="1">
-        <f>AVERAGE(N1_SRC!B8:B9)</f>
-        <v>7.9049999999999994</v>
-      </c>
-      <c r="D2" s="1">
-        <f>AVERAGE(N1_SRC!C8:C9)</f>
-        <v>1.1400000000000001</v>
-      </c>
-      <c r="E2" s="1">
-        <f>AVERAGE(N1_SRC!D8:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <f>AVERAGE(N1_SRC!E8:E9)</f>
-        <v>9.5299999999999994</v>
-      </c>
-      <c r="G2" s="1">
-        <f>AVERAGE(N1_SRC!F8:F9)</f>
-        <v>13.625</v>
-      </c>
-      <c r="H2" s="1">
-        <f>AVERAGE(N1_SRC!G8:G9)</f>
-        <v>13.48</v>
-      </c>
-      <c r="I2" s="1">
-        <f>AVERAGE(N1_SRC!H8:H9)</f>
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>1.9047619047619047</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2690,40 +2788,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <f>AVERAGE(N1_SRC!A11:A12)</f>
-        <v>79.835000000000008</v>
+        <f>AVERAGE(N1_SRC!A8:A9)</f>
+        <v>7.9450000000000003</v>
       </c>
       <c r="C3" s="1">
-        <f>AVERAGE(N1_SRC!B11:B12)</f>
-        <v>78.245000000000005</v>
+        <f>AVERAGE(N1_SRC!B8:B9)</f>
+        <v>7.9049999999999994</v>
       </c>
       <c r="D3" s="1">
-        <f>AVERAGE(N1_SRC!C11:C12)</f>
-        <v>8.8150000000000013</v>
+        <f>AVERAGE(N1_SRC!C8:C9)</f>
+        <v>1.1400000000000001</v>
       </c>
       <c r="E3" s="1">
-        <f>AVERAGE(N1_SRC!D11:D12)</f>
-        <v>7.0950000000000006</v>
+        <f>AVERAGE(N1_SRC!D8:D9)</f>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
-        <f>AVERAGE(N1_SRC!E11:E12)</f>
-        <v>81.655000000000001</v>
+        <f>AVERAGE(N1_SRC!E8:E9)</f>
+        <v>9.5299999999999994</v>
       </c>
       <c r="G3" s="1">
-        <f>AVERAGE(N1_SRC!F11:F12)</f>
-        <v>142.70499999999998</v>
+        <f>AVERAGE(N1_SRC!F8:F9)</f>
+        <v>13.625</v>
       </c>
       <c r="H3" s="1">
-        <f>AVERAGE(N1_SRC!G11:G12)</f>
-        <v>140.94999999999999</v>
+        <f>AVERAGE(N1_SRC!G8:G9)</f>
+        <v>13.48</v>
       </c>
       <c r="I3" s="1">
-        <f>AVERAGE(N1_SRC!H11:H12)</f>
-        <v>12.46</v>
+        <f>AVERAGE(N1_SRC!H8:H9)</f>
+        <v>2.2200000000000002</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1">
-        <v>80</v>
+        <v>1.9047619047619047</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2731,40 +2829,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGE(N1_SRC!A14:A15)</f>
-        <v>341.75</v>
+        <f>AVERAGE(N1_SRC!A11:A12)</f>
+        <v>79.835000000000008</v>
       </c>
       <c r="C4" s="1">
-        <f>AVERAGE(N1_SRC!B14:B15)</f>
-        <v>336.42</v>
+        <f>AVERAGE(N1_SRC!B11:B12)</f>
+        <v>78.245000000000005</v>
       </c>
       <c r="D4" s="1">
-        <f>AVERAGE(N1_SRC!C14:C15)</f>
-        <v>41.064999999999998</v>
+        <f>AVERAGE(N1_SRC!C11:C12)</f>
+        <v>8.8150000000000013</v>
       </c>
       <c r="E4" s="1">
-        <f>AVERAGE(N1_SRC!D14:D15)</f>
-        <v>38.365000000000002</v>
+        <f>AVERAGE(N1_SRC!D11:D12)</f>
+        <v>7.0950000000000006</v>
       </c>
       <c r="F4" s="1">
-        <f>AVERAGE(N1_SRC!E14:E15)</f>
-        <v>420.02499999999998</v>
+        <f>AVERAGE(N1_SRC!E11:E12)</f>
+        <v>81.655000000000001</v>
       </c>
       <c r="G4" s="1">
-        <f>AVERAGE(N1_SRC!F14:F15)</f>
-        <v>678.22</v>
+        <f>AVERAGE(N1_SRC!F11:F12)</f>
+        <v>142.70499999999998</v>
       </c>
       <c r="H4" s="1">
-        <f>AVERAGE(N1_SRC!G14:G15)</f>
-        <v>669.755</v>
+        <f>AVERAGE(N1_SRC!G11:G12)</f>
+        <v>140.94999999999999</v>
       </c>
       <c r="I4" s="1">
-        <f>AVERAGE(N1_SRC!H14:H15)</f>
-        <v>51.924999999999997</v>
+        <f>AVERAGE(N1_SRC!H11:H12)</f>
+        <v>12.46</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1">
-        <v>550</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2772,40 +2870,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGE(N1_SRC!A17:A18)</f>
-        <v>406.20499999999998</v>
+        <f>AVERAGE(N1_SRC!A14:A15)</f>
+        <v>341.75</v>
       </c>
       <c r="C5" s="1">
-        <f>AVERAGE(N1_SRC!B17:B18)</f>
-        <v>397.27</v>
+        <f>AVERAGE(N1_SRC!B14:B15)</f>
+        <v>336.42</v>
       </c>
       <c r="D5" s="1">
-        <f>AVERAGE(N1_SRC!C17:C18)</f>
-        <v>44.980000000000004</v>
+        <f>AVERAGE(N1_SRC!C14:C15)</f>
+        <v>41.064999999999998</v>
       </c>
       <c r="E5" s="1">
-        <f>AVERAGE(N1_SRC!D17:D18)</f>
-        <v>45.855000000000004</v>
+        <f>AVERAGE(N1_SRC!D14:D15)</f>
+        <v>38.365000000000002</v>
       </c>
       <c r="F5" s="1">
-        <f>AVERAGE(N1_SRC!E17:E18)</f>
-        <v>412.16999999999996</v>
+        <f>AVERAGE(N1_SRC!E14:E15)</f>
+        <v>420.02499999999998</v>
       </c>
       <c r="G5" s="1">
-        <f>AVERAGE(N1_SRC!F17:F18)</f>
-        <v>850.14</v>
+        <f>AVERAGE(N1_SRC!F14:F15)</f>
+        <v>678.22</v>
       </c>
       <c r="H5" s="1">
-        <f>AVERAGE(N1_SRC!G17:G18)</f>
-        <v>837.13499999999999</v>
+        <f>AVERAGE(N1_SRC!G14:G15)</f>
+        <v>669.755</v>
       </c>
       <c r="I5" s="1">
-        <f>AVERAGE(N1_SRC!H17:H18)</f>
-        <v>70.045000000000002</v>
+        <f>AVERAGE(N1_SRC!H14:H15)</f>
+        <v>51.924999999999997</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
-        <v>840</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2813,39 +2911,80 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
+        <f>AVERAGE(N1_SRC!A17:A18)</f>
+        <v>406.20499999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(N1_SRC!B17:B18)</f>
+        <v>397.27</v>
+      </c>
+      <c r="D6" s="1">
+        <f>AVERAGE(N1_SRC!C17:C18)</f>
+        <v>44.980000000000004</v>
+      </c>
+      <c r="E6" s="1">
+        <f>AVERAGE(N1_SRC!D17:D18)</f>
+        <v>45.855000000000004</v>
+      </c>
+      <c r="F6" s="1">
+        <f>AVERAGE(N1_SRC!E17:E18)</f>
+        <v>412.16999999999996</v>
+      </c>
+      <c r="G6" s="1">
+        <f>AVERAGE(N1_SRC!F17:F18)</f>
+        <v>850.14</v>
+      </c>
+      <c r="H6" s="1">
+        <f>AVERAGE(N1_SRC!G17:G18)</f>
+        <v>837.13499999999999</v>
+      </c>
+      <c r="I6" s="1">
+        <f>AVERAGE(N1_SRC!H17:H18)</f>
+        <v>70.045000000000002</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <f>AVERAGE(N1_SRC!A20:A21)</f>
         <v>733.18499999999995</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <f>AVERAGE(N1_SRC!B20:B21)</f>
         <v>713.94</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <f>AVERAGE(N1_SRC!C20:C21)</f>
         <v>83.075000000000003</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <f>AVERAGE(N1_SRC!D20:D21)</f>
         <v>79.28</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <f>AVERAGE(N1_SRC!E20:E21)</f>
         <v>749.61500000000001</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
         <f>AVERAGE(N1_SRC!F20:F21)</f>
         <v>3577.3900000000003</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H7" s="1">
         <f>AVERAGE(N1_SRC!G20:G21)</f>
         <v>3526.93</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I7" s="1">
         <f>AVERAGE(N1_SRC!H20:H21)</f>
         <v>634.1099999999999</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
         <v>1492.8571428571427</v>
       </c>
     </row>

</xml_diff>